<commit_message>
Created draft of Final Project report
</commit_message>
<xml_diff>
--- a/Part 1/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/Part 1/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Downloads\FP1.1-350-1201\ensc350-finalproject\Part 1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\Part 1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC94D046-45BD-4DF2-8D93-DA05A3736867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE43D8F5-9788-48B7-B904-F279367D2A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16545" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="50865" yWindow="6465" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Wrote first few entries into activity log. Created a draft of "FPI-Report-G47-350-1202.docx"</t>
+  </si>
+  <si>
+    <t>Updated files from 1.1 to 1.4</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,11 +736,21 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C9" s="9">
+        <v>43923</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.83888888888888891</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>

</xml_diff>

<commit_message>
Part 1: Updated PDF document
</commit_message>
<xml_diff>
--- a/Part 1/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
+++ b/Part 1/Documentation/FP1-log-G47-xxxx-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin-Desktop\Documents\Projects\ensc350-finalproject\Part 1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE43D8F5-9788-48B7-B904-F279367D2A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE920F48-B98C-4EF1-BC6B-0DF31B0B4FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50865" yWindow="6465" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-4155" yWindow="7425" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Updated files from 1.1 to 1.4</t>
+  </si>
+  <si>
+    <t>Updated Final Project PDF document with own name and student number.</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +756,21 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="18"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="11">
+        <v>6977</v>
+      </c>
+      <c r="C10" s="9">
+        <v>43923</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.3430555555555555</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>

</xml_diff>